<commit_message>
Initial report for eel OM
</commit_message>
<xml_diff>
--- a/eel_data_limited_OM.xlsx
+++ b/eel_data_limited_OM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\TNC\Peru MSE\eel MSE\eel-MSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\TNC\Peru MSE\eel MSE\eel_data_limited_OM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46CCB1B-87D7-4620-A520-F44412B4ECA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE0B96D-61D3-492D-93A9-600BC196FE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26412" yWindow="300" windowWidth="17280" windowHeight="11388" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="99">
   <si>
     <t>Slot</t>
   </si>
@@ -308,16 +308,7 @@
     <t>Ebiascv</t>
   </si>
   <si>
-    <t>Generic_Increasing effort</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>Precise-Unbiased</t>
-  </si>
-  <si>
-    <t>Perfect_Imp</t>
+    <t>Data-limited training</t>
   </si>
   <si>
     <t>Common eel</t>
@@ -326,39 +317,23 @@
     <t>Ophichthus remiger</t>
   </si>
   <si>
-    <t>Tumbes, Peru</t>
-  </si>
-  <si>
-    <t>The Nature Conservancy</t>
-  </si>
-  <si>
-    <t>Instituto del Mar del Peru (IMARPE)</t>
+    <t/>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -381,10 +356,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,7 +656,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -700,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -708,15 +683,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>99</v>
+      <c r="B4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -847,10 +822,10 @@
         <v>14</v>
       </c>
       <c r="B17">
+        <v>-2.5499999999999998</v>
+      </c>
+      <c r="C17">
         <v>0.105</v>
-      </c>
-      <c r="C17">
-        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -894,7 +869,7 @@
         <v>0.6</v>
       </c>
       <c r="C21">
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -960,6 +935,9 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +948,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -981,12 +959,12 @@
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -994,15 +972,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
       <c r="B3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1013,58 +991,292 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1990</v>
       </c>
       <c r="C5">
-        <v>0.3</v>
+        <v>1991</v>
       </c>
       <c r="D5">
-        <v>0.6</v>
+        <v>1992</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1993</v>
+      </c>
+      <c r="F5">
+        <v>1994</v>
+      </c>
+      <c r="G5">
+        <v>1995</v>
+      </c>
+      <c r="H5">
+        <v>1996</v>
+      </c>
+      <c r="I5">
+        <v>1997</v>
+      </c>
+      <c r="J5">
+        <v>1998</v>
+      </c>
+      <c r="K5">
+        <v>1999</v>
+      </c>
+      <c r="L5">
+        <v>2000</v>
+      </c>
+      <c r="M5">
+        <v>2001</v>
+      </c>
+      <c r="N5">
+        <v>2002</v>
+      </c>
+      <c r="O5">
+        <v>2003</v>
+      </c>
+      <c r="P5">
+        <v>2004</v>
+      </c>
+      <c r="Q5">
+        <v>2005</v>
+      </c>
+      <c r="R5">
+        <v>2006</v>
+      </c>
+      <c r="S5">
+        <v>2007</v>
+      </c>
+      <c r="T5">
+        <v>2008</v>
+      </c>
+      <c r="U5">
+        <v>2009</v>
+      </c>
+      <c r="V5">
+        <v>2010</v>
+      </c>
+      <c r="W5">
+        <v>2011</v>
+      </c>
+      <c r="X5">
+        <v>2012</v>
+      </c>
+      <c r="Y5">
+        <v>2013</v>
+      </c>
+      <c r="Z5">
+        <v>2014</v>
+      </c>
+      <c r="AA5">
+        <v>2015</v>
+      </c>
+      <c r="AB5">
+        <v>2016</v>
+      </c>
+      <c r="AC5">
+        <v>2017</v>
+      </c>
+      <c r="AD5">
+        <v>2018</v>
+      </c>
+      <c r="AE5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>3.9852200000000003E-3</v>
       </c>
       <c r="C6">
-        <v>0.4</v>
+        <v>4.3581407000000003E-2</v>
       </c>
       <c r="D6">
-        <v>0.4</v>
+        <v>5.9590555000000003E-2</v>
       </c>
       <c r="E6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.1665685000000007E-2</v>
+      </c>
+      <c r="F6">
+        <v>7.9789731000000003E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.115503102</v>
+      </c>
+      <c r="H6">
+        <v>0.123644215</v>
+      </c>
+      <c r="I6">
+        <v>0.13176826</v>
+      </c>
+      <c r="J6">
+        <v>0.104486146</v>
+      </c>
+      <c r="K6">
+        <v>0.14018244999999999</v>
+      </c>
+      <c r="L6">
+        <v>6.1775172000000003E-2</v>
+      </c>
+      <c r="M6">
+        <v>0.21154092299999999</v>
+      </c>
+      <c r="N6">
+        <v>0.361323742</v>
+      </c>
+      <c r="O6">
+        <v>0.66845020200000005</v>
+      </c>
+      <c r="P6">
+        <v>0.80249694900000001</v>
+      </c>
+      <c r="Q6">
+        <v>0.94044357999999995</v>
+      </c>
+      <c r="R6">
+        <v>0.87382128800000003</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0.88223547800000002</v>
+      </c>
+      <c r="U6">
+        <v>0.87070650199999999</v>
+      </c>
+      <c r="V6">
+        <v>0.87096251199999997</v>
+      </c>
+      <c r="W6">
+        <v>0.627343557</v>
+      </c>
+      <c r="X6">
+        <v>0.399426538</v>
+      </c>
+      <c r="Y6">
+        <v>0.486230938</v>
+      </c>
+      <c r="Z6">
+        <v>0.396021607</v>
+      </c>
+      <c r="AA6">
+        <v>0.42776682599999999</v>
+      </c>
+      <c r="AB6">
+        <v>0.428039903</v>
+      </c>
+      <c r="AC6">
+        <v>0.357500661</v>
+      </c>
+      <c r="AD6">
+        <v>0.40104793399999999</v>
+      </c>
+      <c r="AE6">
+        <v>0.38558493999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>3.9852200000000003E-3</v>
       </c>
       <c r="C7">
-        <v>0.6</v>
+        <v>4.3581407000000003E-2</v>
       </c>
       <c r="D7">
-        <v>0.6</v>
+        <v>5.9590555000000003E-2</v>
       </c>
       <c r="E7">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.1665685000000007E-2</v>
+      </c>
+      <c r="F7">
+        <v>7.9789731000000003E-2</v>
+      </c>
+      <c r="G7">
+        <v>0.115503102</v>
+      </c>
+      <c r="H7">
+        <v>0.123644215</v>
+      </c>
+      <c r="I7">
+        <v>0.13176826</v>
+      </c>
+      <c r="J7">
+        <v>0.104486146</v>
+      </c>
+      <c r="K7">
+        <v>0.14018244999999999</v>
+      </c>
+      <c r="L7">
+        <v>6.1775172000000003E-2</v>
+      </c>
+      <c r="M7">
+        <v>0.21154092299999999</v>
+      </c>
+      <c r="N7">
+        <v>0.361323742</v>
+      </c>
+      <c r="O7">
+        <v>0.66845020200000005</v>
+      </c>
+      <c r="P7">
+        <v>0.80249694900000001</v>
+      </c>
+      <c r="Q7">
+        <v>0.94044357999999995</v>
+      </c>
+      <c r="R7">
+        <v>0.87382128800000003</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0.88223547800000002</v>
+      </c>
+      <c r="U7">
+        <v>0.87070650199999999</v>
+      </c>
+      <c r="V7">
+        <v>0.87096251199999997</v>
+      </c>
+      <c r="W7">
+        <v>0.627343557</v>
+      </c>
+      <c r="X7">
+        <v>0.399426538</v>
+      </c>
+      <c r="Y7">
+        <v>0.486230938</v>
+      </c>
+      <c r="Z7">
+        <v>0.396021607</v>
+      </c>
+      <c r="AA7">
+        <v>0.42776682599999999</v>
+      </c>
+      <c r="AB7">
+        <v>0.428039903</v>
+      </c>
+      <c r="AC7">
+        <v>0.357500661</v>
+      </c>
+      <c r="AD7">
+        <v>0.40104793399999999</v>
+      </c>
+      <c r="AE7">
+        <v>0.38558493999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1075,7 +1287,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1086,7 +1298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1097,48 +1309,48 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11">
-        <v>0.2</v>
+        <v>28.3</v>
       </c>
       <c r="C11">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
       <c r="B12">
-        <v>0.75</v>
+        <v>42</v>
       </c>
       <c r="C12">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1149,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1187,7 +1399,7 @@
         <v>44</v>
       </c>
       <c r="B19">
-        <v>50</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1227,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1522,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1602,13 +1814,12 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1627,29 +1838,20 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1706,7 +1908,7 @@
         <v>88</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>